<commit_message>
PA01 - Test Cases
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/PA1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josecarrillo/PycharmProjects/HOLA/cs151-pa1-Jose-Carrillo38/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0D32F8-6D7A-7B45-9670-B8699C8948C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7330C6-EC16-7B4E-9CC5-2ACA97B03FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67920" windowHeight="28300" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-37100" yWindow="-3100" windowWidth="21620" windowHeight="16240" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,17 +34,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>You need to create your own tests</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Choice1</t>
+  </si>
+  <si>
+    <t>Choice3</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>2 (Tree height: 20)</t>
+  </si>
+  <si>
+    <t>2 (Tree height: 10)</t>
+  </si>
+  <si>
+    <t>Speed: 25</t>
+  </si>
+  <si>
+    <t>Speed: 15</t>
+  </si>
+  <si>
+    <t>Choice2 (Ft/MPH)</t>
+  </si>
+  <si>
+    <t>Player throws rocks, climbs a short tree, is caught by the bear, and the game ends</t>
+  </si>
+  <si>
+    <t>Player throws rocks, tries to run, is caught by the bear, and ends up at the bear's cabin</t>
+  </si>
+  <si>
+    <t>Player throws rocks, tries to run, is caught by the bear, but escapes the forest by taking the right path</t>
+  </si>
+  <si>
+    <t>Player throws rocks, climbs a tall tree, avoids the bear, but ends up at the bear's cabin</t>
+  </si>
+  <si>
+    <t>Player throws rocks, climbs a tall tree, avoids the bear, and escapes the forest by taking the right path</t>
+  </si>
+  <si>
+    <t>Player runs quickly, outruns the bear, but ends up at the bear's cabin</t>
+  </si>
+  <si>
+    <t>Player runs quickly, outruns the bear, and escapes the forest by taking the right path</t>
+  </si>
+  <si>
+    <t>Player tries to run but is caught by the bear, and the game ends</t>
+  </si>
+  <si>
+    <t>Player stays still, bear loses interest, but ends up at the bear's cabin after taking the left path</t>
+  </si>
+  <si>
+    <t>Player stays still, bear loses interest, and escapes the forest by taking the right path</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,10 +140,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -391,26 +465,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF6E1F2-B43E-D343-BB9B-DE90F40B65C5}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="84.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="80" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>